<commit_message>
Updated the hard-coded files path to System path
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rganjare/eclipse/WorkSpace/SeleniumTraining_B14_MVN/src/test/resources/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\OnlineTraining\SeleniumTraining_B14_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87272ABE-DEAD-AA46-8418-4E53E94266C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349EF030-3FB4-4192-9379-A861FD1BCA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="1" r:id="rId1"/>
@@ -606,22 +606,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.83203125" style="2" collapsed="1"/>
-    <col min="6" max="6" width="8.83203125" style="2"/>
-    <col min="7" max="16384" width="8.83203125" style="2" collapsed="1"/>
+    <col min="1" max="1" width="11.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.6328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.81640625" style="2" collapsed="1"/>
+    <col min="6" max="6" width="8.81640625" style="2"/>
+    <col min="7" max="16384" width="8.81640625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -663,7 +663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -677,7 +677,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -705,7 +705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -719,7 +719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -733,7 +733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -747,7 +747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -761,7 +761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -775,7 +775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -805,29 +805,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668CBAB-C452-40CE-A283-6DB616929218}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="76.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2" collapsed="1"/>
+    <col min="1" max="1" width="8.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.6328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="76.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="8.81640625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -853,7 +853,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -879,12 +879,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -910,7 +910,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -936,7 +936,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -962,7 +962,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -988,12 +988,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1045,12 +1045,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
@@ -1102,12 +1102,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1159,12 +1159,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
@@ -1210,12 +1210,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" s="6" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Added changes for Jenkins job
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\OnlineTraining\SeleniumTraining_B14_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349EF030-3FB4-4192-9379-A861FD1BCA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2262FB48-781F-44D8-8193-DA1F466EDF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="1" r:id="rId1"/>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668CBAB-C452-40CE-A283-6DB616929218}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="21" x14ac:dyDescent="0.5"/>

</xml_diff>